<commit_message>
Added Class Articles md file
</commit_message>
<xml_diff>
--- a/Excel/Excel-Test-1.xlsx
+++ b/Excel/Excel-Test-1.xlsx
@@ -105,9 +105,6 @@
     <t>(fill in January to July automatically)</t>
   </si>
   <si>
-    <t>3. Pull in the January to July sales month names and sales (using relative reference) from the previous sheet.</t>
-  </si>
-  <si>
     <t xml:space="preserve">4. Calculate the tax for each month using an absolute reference back to the Sales Tax number on sheet 1. </t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t xml:space="preserve">8. Format all dollar values with two decimal places and a left-aligned dollar sign. </t>
+  </si>
+  <si>
+    <t>3. Pull in the January to July month names and sales (using relative references) from the previous sheet.</t>
   </si>
 </sst>
 </file>
@@ -249,6 +249,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -261,38 +288,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,12 +587,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -601,34 +601,34 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17">
+      <c r="A4" s="11"/>
+      <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17">
+      <c r="A5" s="11"/>
+      <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17">
+      <c r="A6" s="11"/>
+      <c r="B6" s="5">
         <v>4</v>
       </c>
       <c r="D6" s="2"/>
@@ -636,235 +636,230 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17">
+      <c r="A7" s="11"/>
+      <c r="B7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17">
+      <c r="A8" s="11"/>
+      <c r="B8" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17">
+      <c r="A9" s="11"/>
+      <c r="B9" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17">
+      <c r="A10" s="11"/>
+      <c r="B10" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17">
+      <c r="A11" s="11"/>
+      <c r="B11" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="17">
+      <c r="A12" s="11"/>
+      <c r="B12" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="5"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="5" t="str">
+      <c r="B14" s="7"/>
+      <c r="C14" s="16" t="str">
         <f>+C13</f>
         <v>(must use named range)</v>
       </c>
-      <c r="D14" s="5"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="9" t="s">
+      <c r="A15" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="9"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="19"/>
+      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="19"/>
+      <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="7"/>
+      <c r="C22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="6"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="19"/>
+      <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="19"/>
+      <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="7" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="18"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="19"/>
+      <c r="B26" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="15" t="s">
+      <c r="A30" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
+      <c r="A31" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="19">
+      <c r="B31" s="7">
         <v>0.13</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="8"/>
+      <c r="D31" s="19"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="19"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="19">
+      <c r="B33" s="7">
         <v>20297</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="5"/>
+      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="19">
+      <c r="A34" s="8"/>
+      <c r="B34" s="7">
         <v>17392</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="19">
+      <c r="A35" s="8"/>
+      <c r="B35" s="7">
         <v>25408</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="19">
+      <c r="A36" s="8"/>
+      <c r="B36" s="7">
         <v>15343</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="19">
+      <c r="A37" s="8"/>
+      <c r="B37" s="7">
         <v>13568</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-      <c r="B38" s="19">
+      <c r="A38" s="8"/>
+      <c r="B38" s="7">
         <v>29266</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
+      <c r="A39" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="19">
+      <c r="B39" s="7">
         <v>27644</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -873,6 +868,11 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C15:D19"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -887,7 +887,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,12 +896,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
+      <c r="A1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -910,140 +910,140 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-    </row>
-    <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+    </row>
+    <row r="9" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-    </row>
-    <row r="7" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-    </row>
-    <row r="9" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-    </row>
-    <row r="10" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="20" t="s">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="19"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="19"/>
+      <c r="D22" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Final Edit for today
Need to consult the students to see if they want anything else in the test.
</commit_message>
<xml_diff>
--- a/Excel/Excel-Test-1.xlsx
+++ b/Excel/Excel-Test-1.xlsx
@@ -9,12 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="RandFloat">Sheet2!$A$162</definedName>
+    <definedName name="RandInt">Sheet2!$A$163</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Name this range "Nums1-10":</t>
   </si>
@@ -99,9 +103,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Continued on Sheet 2…</t>
-  </si>
-  <si>
     <t>(fill in January to July automatically)</t>
   </si>
   <si>
@@ -142,13 +143,34 @@
   </si>
   <si>
     <t>3. Pull in the January to July month names and sales (using relative references) from the previous sheet.</t>
+  </si>
+  <si>
+    <t>Continued on Sheet 2 (Part C)…</t>
+  </si>
+  <si>
+    <t>Part D</t>
+  </si>
+  <si>
+    <t>2. In it, put:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total sales are: </t>
+  </si>
+  <si>
+    <t>1. Create a separate Excel file called "Total-Sales".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…where the total sales value is pulled in from this Excel file (cell D21). </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +194,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +225,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -235,10 +277,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -264,18 +307,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -288,14 +319,41 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -576,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A25" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,12 +645,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -601,7 +659,7 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5">
@@ -609,25 +667,25 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="19"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -636,37 +694,37 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -676,55 +734,55 @@
         <v>1</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="16"/>
+      <c r="D13" s="12"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="16" t="str">
+      <c r="C14" s="12" t="str">
         <f>+C13</f>
         <v>(must use named range)</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>33</v>
+      <c r="A15" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="20"/>
+      <c r="C15" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="11"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -743,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="13"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -765,10 +823,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="18"/>
+      <c r="D25" s="14"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -777,12 +835,12 @@
       <c r="B26" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
@@ -791,75 +849,87 @@
       <c r="B31" s="7">
         <v>0.13</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="19"/>
+      <c r="D31" s="15"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="7">
-        <v>20297</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D33" s="16"/>
+      <c r="B33" s="23">
+        <f ca="1">RANDBETWEEN(10000, 100000)</f>
+        <v>87029</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D33" s="12"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="7">
-        <v>17392</v>
+      <c r="A34" s="24"/>
+      <c r="B34" s="23">
+        <f t="shared" ref="B34:B39" ca="1" si="0">RANDBETWEEN(10000, 100000)</f>
+        <v>50699</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="7">
-        <v>25408</v>
+      <c r="A35" s="24"/>
+      <c r="B35" s="23">
+        <f t="shared" ca="1" si="0"/>
+        <v>52905</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="7">
-        <v>15343</v>
+      <c r="A36" s="24"/>
+      <c r="B36" s="23">
+        <f t="shared" ca="1" si="0"/>
+        <v>80384</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="7">
-        <v>13568</v>
+      <c r="A37" s="24"/>
+      <c r="B37" s="23">
+        <f t="shared" ca="1" si="0"/>
+        <v>55663</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="7">
-        <v>29266</v>
+      <c r="A38" s="24"/>
+      <c r="B38" s="23">
+        <f t="shared" ca="1" si="0"/>
+        <v>93345</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="7">
-        <v>27644</v>
+      <c r="B39" s="23">
+        <f t="shared" ca="1" si="0"/>
+        <v>25814</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
+      <c r="A41" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -868,11 +938,6 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C15:D19"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -884,10 +949,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,12 +961,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="A1" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -909,69 +974,69 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-    </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1033,7 +1098,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="7"/>
     </row>
@@ -1041,12 +1106,52 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="7"/>
     </row>
+    <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="26"/>
+      <c r="C30" s="28">
+        <v>234563.45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="27"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="11">
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A30:B30"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>

</xml_diff>

<commit_message>
Minor update to test
</commit_message>
<xml_diff>
--- a/Excel/Excel-Test-1.xlsx
+++ b/Excel/Excel-Test-1.xlsx
@@ -121,9 +121,6 @@
     <t xml:space="preserve">7. Format any totals that are below the sales average in a red font. Use conditional formatting for this. </t>
   </si>
   <si>
-    <t>2. Put a double underline under the headings.</t>
-  </si>
-  <si>
     <t>Format the cells in RandNums so the negative numbers are red with no negative sign.</t>
   </si>
   <si>
@@ -161,6 +158,9 @@
   </si>
   <si>
     <t xml:space="preserve">…where the total sales value is pulled in from this Excel file (cell D21). </t>
+  </si>
+  <si>
+    <t>2. Put a double underline under the headings. (not the double border)</t>
   </si>
 </sst>
 </file>
@@ -307,6 +307,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -319,38 +342,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -645,12 +645,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -659,7 +659,7 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5">
@@ -667,25 +667,25 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="17"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -694,37 +694,37 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -734,55 +734,55 @@
         <v>1</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="12" t="str">
+      <c r="C14" s="21" t="str">
         <f>+C13</f>
         <v>(must use named range)</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>32</v>
+      <c r="A15" s="16" t="s">
+        <v>31</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="16"/>
+      <c r="C15" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="17"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -801,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="13"/>
+      <c r="D22" s="22"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -823,10 +823,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="14"/>
+      <c r="D25" s="23"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -835,12 +835,12 @@
       <c r="B26" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
@@ -849,87 +849,82 @@
       <c r="B31" s="7">
         <v>0.13</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="15"/>
+      <c r="D31" s="24"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="23">
+      <c r="B33" s="11">
         <f ca="1">RANDBETWEEN(10000, 100000)</f>
-        <v>87029</v>
-      </c>
-      <c r="C33" s="12" t="s">
+        <v>76424</v>
+      </c>
+      <c r="C33" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="23">
+      <c r="A34" s="12"/>
+      <c r="B34" s="11">
         <f t="shared" ref="B34:B39" ca="1" si="0">RANDBETWEEN(10000, 100000)</f>
-        <v>50699</v>
+        <v>49405</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="23">
+      <c r="A35" s="12"/>
+      <c r="B35" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>52905</v>
+        <v>74879</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="24"/>
-      <c r="B36" s="23">
+      <c r="A36" s="12"/>
+      <c r="B36" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>80384</v>
+        <v>74491</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="24"/>
-      <c r="B37" s="23">
+      <c r="A37" s="12"/>
+      <c r="B37" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>55663</v>
+        <v>63738</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="24"/>
-      <c r="B38" s="23">
+      <c r="A38" s="12"/>
+      <c r="B38" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>93345</v>
+        <v>85691</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="23">
+      <c r="B39" s="11">
         <f t="shared" ca="1" si="0"/>
-        <v>25814</v>
+        <v>76706</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
+      <c r="A41" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -938,6 +933,11 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C15:D19"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,12 +961,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -975,68 +975,68 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-    </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-    </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1111,41 +1111,41 @@
       <c r="D22" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="A25" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="26"/>
-      <c r="C30" s="28">
+      <c r="C30" s="15">
         <v>234563.45</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="27"/>
+      <c r="C31" s="14"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a demo showing how to link to another Excel file
Created files. Video and ReadMe to follow.
</commit_message>
<xml_diff>
--- a/Excel/Excel-Test-1.xlsx
+++ b/Excel/Excel-Test-1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -167,8 +167,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -307,9 +308,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -318,18 +316,6 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -342,6 +328,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -350,6 +348,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -634,23 +635,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -659,7 +661,7 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="5">
@@ -667,25 +669,25 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="21"/>
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="23" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="21"/>
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="21"/>
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -694,37 +696,37 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="21"/>
       <c r="B7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="21"/>
       <c r="B8" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="21"/>
       <c r="B9" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="21"/>
       <c r="B10" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="16"/>
+      <c r="A11" s="21"/>
       <c r="B11" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -734,55 +736,55 @@
         <v>1</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="21"/>
+      <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="21" t="str">
+      <c r="C14" s="16" t="str">
         <f>+C13</f>
         <v>(must use named range)</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="21" t="s">
         <v>31</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="25"/>
+      <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="A16" s="21"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="21"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="21"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -801,10 +803,10 @@
         <v>6</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="22"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
@@ -823,10 +825,10 @@
         <v>12</v>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="23"/>
+      <c r="D25" s="18"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
@@ -835,12 +837,12 @@
       <c r="B26" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="19" t="s">
+      <c r="A30" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
@@ -849,82 +851,87 @@
       <c r="B31" s="7">
         <v>0.13</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="24"/>
+      <c r="D31" s="19"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="7"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="11">
-        <f ca="1">RANDBETWEEN(10000, 100000)</f>
-        <v>76424</v>
-      </c>
-      <c r="C33" s="21" t="s">
+      <c r="B33" s="28">
+        <f ca="1">RANDBETWEEN(10000, 100000)*RAND()</f>
+        <v>50637.334736125493</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="21"/>
+      <c r="D33" s="16"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="11">
-        <f t="shared" ref="B34:B39" ca="1" si="0">RANDBETWEEN(10000, 100000)</f>
-        <v>49405</v>
+      <c r="A34" s="11"/>
+      <c r="B34" s="28">
+        <f t="shared" ref="B34:B39" ca="1" si="0">RANDBETWEEN(10000, 100000)*RAND()</f>
+        <v>83296.339994707349</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="11">
+      <c r="A35" s="11"/>
+      <c r="B35" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>74879</v>
+        <v>68762.047569747869</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
-      <c r="B36" s="11">
+      <c r="A36" s="11"/>
+      <c r="B36" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>74491</v>
+        <v>25845.185201804721</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
-      <c r="B37" s="11">
+      <c r="A37" s="11"/>
+      <c r="B37" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>63738</v>
+        <v>53241.564856059267</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
-      <c r="B38" s="11">
+      <c r="A38" s="11"/>
+      <c r="B38" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>85691</v>
+        <v>29050.657961866305</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>76706</v>
+        <v>55719.831913858761</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
@@ -933,11 +940,6 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C15:D19"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -951,7 +953,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D4"/>
     </sheetView>
   </sheetViews>
@@ -961,12 +963,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -975,68 +977,68 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
     </row>
     <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -1111,12 +1113,12 @@
       <c r="D22" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1130,18 +1132,18 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+      <c r="A30" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B30" s="26"/>
-      <c r="C30" s="15">
+      <c r="B30" s="25"/>
+      <c r="C30" s="14">
         <v>234563.45</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="14"/>
+      <c r="C31" s="13"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">

</xml_diff>

<commit_message>
Had to fix one of the named range requirements.
Can't include hyphens apparently!
</commit_message>
<xml_diff>
--- a/Excel/Excel-Test-1.xlsx
+++ b/Excel/Excel-Test-1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8040"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,15 +31,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
-    <t>Name this range "Nums1-10":</t>
-  </si>
-  <si>
-    <t>Sum of Nums1-10:</t>
-  </si>
-  <si>
-    <t>Average of Nums1-10:</t>
-  </si>
-  <si>
     <t>Max of RandNums:</t>
   </si>
   <si>
@@ -154,13 +145,22 @@
     <t xml:space="preserve">The total sales are: </t>
   </si>
   <si>
-    <t>1. Create a separate Excel file called "Total-Sales".</t>
-  </si>
-  <si>
     <t xml:space="preserve">…where the total sales value is pulled in from this Excel file (cell D21). </t>
   </si>
   <si>
     <t>2. Put a double underline under the headings. (not the double border)</t>
+  </si>
+  <si>
+    <t>1. Create a separate Excel file called "TotalSales".</t>
+  </si>
+  <si>
+    <t>Name this range "Nums1_10":</t>
+  </si>
+  <si>
+    <t>Sum of Nums1_10:</t>
+  </si>
+  <si>
+    <t>Average of Nums1_10:</t>
   </si>
 </sst>
 </file>
@@ -316,6 +316,9 @@
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -348,9 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
-      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -636,7 +636,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="A15" sqref="A15:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,12 +647,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -661,33 +661,33 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>0</v>
+      <c r="A3" s="22" t="s">
+        <v>41</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="22"/>
       <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>11</v>
+      <c r="D4" s="24" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -696,165 +696,165 @@
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
+      <c r="A11" s="22"/>
       <c r="B11" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B13" s="7"/>
-      <c r="C13" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="16"/>
+      <c r="C13" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="16" t="str">
+      <c r="C14" s="17" t="str">
         <f>+C13</f>
         <v>(must use named range)</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="17"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>31</v>
+      <c r="A15" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="20"/>
+      <c r="C15" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="5"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
+      <c r="A17" s="22"/>
       <c r="B17" s="5"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="5"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" s="7"/>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B22" s="7"/>
-      <c r="C22" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="17"/>
+      <c r="C22" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="18"/>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B23" s="7"/>
     </row>
     <row r="24" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B24" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="18"/>
+      <c r="C25" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="19"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="22"/>
+      <c r="A30" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B31" s="7">
         <v>0.13</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="19"/>
+      <c r="C31" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="20"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
@@ -862,68 +862,68 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B33" s="28">
+        <v>15</v>
+      </c>
+      <c r="B33" s="15">
         <f ca="1">RANDBETWEEN(10000, 100000)*RAND()</f>
-        <v>50637.334736125493</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D33" s="16"/>
+        <v>11364.782162475905</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="17"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
-      <c r="B34" s="28">
+      <c r="B34" s="15">
         <f t="shared" ref="B34:B39" ca="1" si="0">RANDBETWEEN(10000, 100000)*RAND()</f>
-        <v>83296.339994707349</v>
+        <v>47094.394458130293</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
-      <c r="B35" s="28">
+      <c r="B35" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>68762.047569747869</v>
+        <v>42144.044821050586</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
-      <c r="B36" s="28">
+      <c r="B36" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>25845.185201804721</v>
+        <v>11704.657303808657</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
-      <c r="B37" s="28">
+      <c r="B37" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>53241.564856059267</v>
+        <v>45774.609282638339</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
-      <c r="B38" s="28">
+      <c r="B38" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>29050.657961866305</v>
+        <v>32189.942928070745</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B39" s="28">
+        <v>16</v>
+      </c>
+      <c r="B39" s="15">
         <f t="shared" ca="1" si="0"/>
-        <v>55719.831913858761</v>
+        <v>1981.5260652096672</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
+      <c r="A41" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="16"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -953,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,12 +963,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
@@ -977,81 +977,81 @@
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+    </row>
+    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="27"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+    </row>
+    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-    </row>
-    <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-    </row>
-    <row r="5" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-    </row>
-    <row r="6" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-    </row>
-    <row r="7" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-    </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-    </row>
-    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-    </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1100,7 +1100,7 @@
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D21" s="7"/>
     </row>
@@ -1108,34 +1108,34 @@
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D22" s="7"/>
     </row>
     <row r="25" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
+      <c r="A25" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="25"/>
+      <c r="A30" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="26"/>
       <c r="C30" s="14">
         <v>234563.45</v>
       </c>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>